<commit_message>
working on runing medium instances
</commit_message>
<xml_diff>
--- a/hw1/Instances/Results.xlsx
+++ b/hw1/Instances/Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FD1821-23E2-463E-AA26-19975A6C358F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F8B6DA-7BE6-4521-B647-6491A2B1ED42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1176" windowWidth="9180" windowHeight="7524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7260" yWindow="2088" windowWidth="12312" windowHeight="9396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>br17.1.sop</t>
   </si>
@@ -269,13 +269,130 @@
   </si>
   <si>
     <t>83310.0</t>
+  </si>
+  <si>
+    <t>2643.1</t>
+  </si>
+  <si>
+    <t>2619.2</t>
+  </si>
+  <si>
+    <t>394.5</t>
+  </si>
+  <si>
+    <t>387.0</t>
+  </si>
+  <si>
+    <t>2048.4</t>
+  </si>
+  <si>
+    <t>2140.4</t>
+  </si>
+  <si>
+    <t>1765.7</t>
+  </si>
+  <si>
+    <t>1761.8</t>
+  </si>
+  <si>
+    <t>435.7</t>
+  </si>
+  <si>
+    <t>411.0</t>
+  </si>
+  <si>
+    <t>481.3</t>
+  </si>
+  <si>
+    <t>1085.1</t>
+  </si>
+  <si>
+    <t>1468.1</t>
+  </si>
+  <si>
+    <t>1407.0</t>
+  </si>
+  <si>
+    <t>1427.5</t>
+  </si>
+  <si>
+    <t>2631.9</t>
+  </si>
+  <si>
+    <t>3155.7</t>
+  </si>
+  <si>
+    <t>3163.4</t>
+  </si>
+  <si>
+    <t>19296.9</t>
+  </si>
+  <si>
+    <t>23702.9</t>
+  </si>
+  <si>
+    <t>1886.1</t>
+  </si>
+  <si>
+    <t>1075.1</t>
+  </si>
+  <si>
+    <t>1510.5</t>
+  </si>
+  <si>
+    <t>1808.5</t>
+  </si>
+  <si>
+    <t>2097.6</t>
+  </si>
+  <si>
+    <t>2307.3</t>
+  </si>
+  <si>
+    <t>3606.8</t>
+  </si>
+  <si>
+    <t>3009.2</t>
+  </si>
+  <si>
+    <t>173.2</t>
+  </si>
+  <si>
+    <t>46949.9</t>
+  </si>
+  <si>
+    <t>583.0</t>
+  </si>
+  <si>
+    <t>806.4</t>
+  </si>
+  <si>
+    <t>252.8</t>
+  </si>
+  <si>
+    <t>1034.4</t>
+  </si>
+  <si>
+    <t>159.6</t>
+  </si>
+  <si>
+    <t>69.4</t>
+  </si>
+  <si>
+    <t>85.5</t>
+  </si>
+  <si>
+    <t>132.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-3000401]#,##0.00"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +422,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -326,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,6 +468,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -771,7 +899,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
@@ -791,7 +919,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2">
@@ -851,11 +979,23 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>1123</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2372</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2201</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -865,24 +1005,60 @@
       <c r="B14" s="2">
         <v>243</v>
       </c>
+      <c r="C14" s="3">
+        <v>346</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="2">
+        <v>353</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>1071</v>
       </c>
+      <c r="C15" s="3">
+        <v>1699</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1714</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>912</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <v>1625</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1610</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -890,175 +1066,298 @@
         <v>879</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>400</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <v>411</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>397</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <v>404</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>467</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E20" s="2">
+        <v>469</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>1023</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E21" s="2">
+        <v>1047</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2">
         <v>1423</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E22" s="2">
+        <v>1437</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>1361</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E23" s="2">
+        <v>1369</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>1381</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E24" s="2">
+        <v>1390</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="2">
         <v>1765</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E25" s="2">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>2544</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E26" s="2">
+        <v>2581</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="2">
         <v>3062</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E27" s="2">
+        <v>3138</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="2">
         <v>2568</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E28" s="2">
+        <v>3125</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="2">
         <v>16666</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E29" s="2">
+        <v>18247</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>19894</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="E30" s="2">
+        <v>21773</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="2">
         <v>915</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="E31" s="2">
+        <v>1598</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="2">
         <v>198</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E32" s="2">
+        <v>1050</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>56</v>
       </c>
       <c r="B33" s="2">
         <v>1494</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E33" s="2">
+        <v>1497</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="2">
         <v>1750</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E34" s="2">
+        <v>1782</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="2">
         <v>2033</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E35" s="2">
+        <v>2062</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="2">
         <v>2241</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E36" s="2">
+        <v>2283</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
       <c r="B37" s="2">
         <v>3482</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E37" s="2">
+        <v>3561</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>61</v>
       </c>
       <c r="B38" s="2">
         <v>2545</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E38" s="2">
+        <v>2922</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -1066,55 +1365,91 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="2">
         <v>577</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E41" s="2">
+        <v>580</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
       <c r="B42" s="2">
         <v>791</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E42" s="2">
+        <v>797</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="2">
         <v>245</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E43" s="2">
+        <v>247</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
       <c r="B44" s="2">
         <v>1016</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E44" s="2">
+        <v>1022</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
       <c r="B45" s="2">
         <v>155</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E45" s="2">
+        <v>155</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
       <c r="B46" s="2">
         <v>64</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E46" s="2">
+        <v>65</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -1122,7 +1457,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -1130,31 +1465,49 @@
         <v>3466</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
       <c r="B49" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E49" s="2">
+        <v>84</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
       <c r="B50" s="2">
         <v>127</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E50" s="2">
+        <v>127</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>38</v>
       </c>
       <c r="B52" s="2">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E52" s="2">
+        <v>154</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -1162,15 +1515,21 @@
         <v>71749</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>40</v>
       </c>
       <c r="B54" s="2">
         <v>41196</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E54" s="2">
+        <v>45481</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>41</v>
       </c>
@@ -1178,7 +1537,7 @@
         <v>71556</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -1186,7 +1545,7 @@
         <v>109471</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -1194,7 +1553,7 @@
         <v>38963</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>44</v>
       </c>
@@ -1202,7 +1561,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>45</v>
       </c>
@@ -1210,7 +1569,7 @@
         <v>23293</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>46</v>
       </c>
@@ -1218,7 +1577,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>47</v>
       </c>
@@ -1226,7 +1585,7 @@
         <v>214608</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -1234,7 +1593,7 @@
         <v>65678</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
plot and timer function added
</commit_message>
<xml_diff>
--- a/hw1/Instances/Results.xlsx
+++ b/hw1/Instances/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3749B84B-1AAD-4EE3-8D2C-1580472FCB5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DD7B84-35C8-4E5E-8D9B-C64FB34F1C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7260" yWindow="2088" windowWidth="12312" windowHeight="9396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
   <si>
     <t>br17.1.sop</t>
   </si>
@@ -403,7 +403,37 @@
     <t>66523.0</t>
   </si>
   <si>
-    <t>toooo long</t>
+    <t>3745.7</t>
+  </si>
+  <si>
+    <t>24577.2</t>
+  </si>
+  <si>
+    <t>42.3</t>
+  </si>
+  <si>
+    <t>max_exp</t>
+  </si>
+  <si>
+    <t>59.4</t>
+  </si>
+  <si>
+    <t>59.2</t>
+  </si>
+  <si>
+    <t>18558.0</t>
+  </si>
+  <si>
+    <t>max_log</t>
+  </si>
+  <si>
+    <t>2002.8</t>
+  </si>
+  <si>
+    <t>73565.4</t>
+  </si>
+  <si>
+    <t>225826.7</t>
   </si>
 </sst>
 </file>
@@ -471,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -494,6 +524,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -786,10 +819,11 @@
     <col min="1" max="1" width="20.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.09765625" style="2"/>
     <col min="3" max="3" width="8.796875" style="3"/>
-    <col min="4" max="6" width="8.796875" style="2"/>
+    <col min="4" max="7" width="8.796875" style="2"/>
+    <col min="8" max="8" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -802,14 +836,20 @@
       <c r="D1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -822,8 +862,17 @@
       <c r="D2" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="2">
+        <v>41</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -836,8 +885,17 @@
       <c r="D3" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>55</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -850,8 +908,17 @@
       <c r="D4" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="2">
+        <v>55</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -864,8 +931,17 @@
       <c r="D5" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2">
+        <v>18325</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" s="3">
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -878,8 +954,17 @@
       <c r="D6" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <v>2125</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -892,14 +977,14 @@
       <c r="D7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>9581</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -912,14 +997,14 @@
       <c r="D8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>44128</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -932,14 +1017,14 @@
       <c r="D9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>46859</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -952,14 +1037,14 @@
       <c r="D10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>58699</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -972,14 +1057,14 @@
       <c r="D11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>28305</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -992,14 +1077,14 @@
       <c r="D12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>83170</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1012,14 +1097,14 @@
       <c r="D13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>2201</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1032,14 +1117,14 @@
       <c r="D14" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>353</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -1052,14 +1137,14 @@
       <c r="D15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>1714</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
@@ -1072,583 +1157,619 @@
       <c r="D16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>1610</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>879</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="2">
+        <v>1757</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" s="3">
+        <v>2235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>400</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>411</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>397</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>404</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>467</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>469</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>1023</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="2">
         <v>1047</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2">
         <v>1423</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>1437</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>1361</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>1369</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>1381</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>1390</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="2">
         <v>1765</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="2">
         <v>1793</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>2544</v>
       </c>
-      <c r="E26" s="2">
+      <c r="F26" s="2">
         <v>2581</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="2">
         <v>3062</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="2">
         <v>3138</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="2">
         <v>2568</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="2">
         <v>3125</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="2">
         <v>16666</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>18247</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>19894</v>
       </c>
-      <c r="E30" s="2">
+      <c r="F30" s="2">
         <v>21773</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="2">
         <v>915</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="2">
         <v>1598</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="2">
         <v>198</v>
       </c>
-      <c r="E32" s="2">
+      <c r="F32" s="2">
         <v>1050</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>56</v>
       </c>
       <c r="B33" s="2">
         <v>1494</v>
       </c>
-      <c r="E33" s="2">
+      <c r="F33" s="2">
         <v>1497</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="2">
         <v>1750</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="2">
         <v>1782</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="2">
         <v>2033</v>
       </c>
-      <c r="E35" s="2">
+      <c r="F35" s="2">
         <v>2062</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="2">
         <v>2241</v>
       </c>
-      <c r="E36" s="2">
+      <c r="F36" s="2">
         <v>2283</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
       <c r="B37" s="2">
         <v>3482</v>
       </c>
-      <c r="E37" s="2">
+      <c r="F37" s="2">
         <v>3561</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>61</v>
       </c>
       <c r="B38" s="2">
         <v>2545</v>
       </c>
-      <c r="E38" s="2">
+      <c r="F38" s="2">
         <v>2922</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>29</v>
       </c>
       <c r="B40" s="2">
         <v>1109</v>
       </c>
-      <c r="E40" s="2">
+      <c r="F40" s="2">
         <v>1111</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="2">
         <v>577</v>
       </c>
-      <c r="E41" s="2">
+      <c r="F41" s="2">
         <v>580</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
       <c r="B42" s="2">
         <v>791</v>
       </c>
-      <c r="E42" s="2">
+      <c r="F42" s="2">
         <v>797</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="2">
         <v>245</v>
       </c>
-      <c r="E43" s="2">
+      <c r="F43" s="2">
         <v>247</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
       <c r="B44" s="2">
         <v>1016</v>
       </c>
-      <c r="E44" s="2">
+      <c r="F44" s="2">
         <v>1022</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
       <c r="B45" s="2">
         <v>155</v>
       </c>
-      <c r="E45" s="2">
+      <c r="F45" s="2">
         <v>155</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
       <c r="B46" s="2">
         <v>64</v>
       </c>
-      <c r="E46" s="2">
+      <c r="F46" s="2">
         <v>65</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
       <c r="B47" s="2">
         <v>2018</v>
       </c>
-      <c r="E47" s="2">
+      <c r="F47" s="2">
         <v>2018</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
       <c r="B48" s="2">
         <v>3466</v>
       </c>
-      <c r="E48" s="2">
+      <c r="F48" s="2">
         <v>3466</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
       <c r="B49" s="2">
         <v>84</v>
       </c>
-      <c r="E49" s="2">
+      <c r="F49" s="2">
         <v>84</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
       <c r="B50" s="2">
         <v>127</v>
       </c>
-      <c r="E50" s="2">
+      <c r="F50" s="2">
         <v>127</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>38</v>
       </c>
       <c r="B52" s="2">
         <v>61</v>
       </c>
-      <c r="E52" s="2">
+      <c r="F52" s="2">
         <v>154</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
       <c r="B53" s="2">
         <v>71749</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F53" s="2">
+        <v>73090</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H53" s="3">
+        <v>74322</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>40</v>
       </c>
       <c r="B54" s="2">
         <v>41196</v>
       </c>
-      <c r="E54" s="2">
+      <c r="F54" s="2">
         <v>45481</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="G54" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="2">
         <v>71556</v>
       </c>
-      <c r="E55" s="2">
+      <c r="F55" s="2">
         <v>72943</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="2">
         <v>109471</v>
       </c>
-      <c r="E56" s="2">
+      <c r="F56" s="2">
         <v>112435</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B57" s="2">
         <v>38963</v>
       </c>
-      <c r="E57" s="2">
+      <c r="F57" s="2">
         <v>63323</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>44</v>
       </c>
       <c r="B58" s="2">
         <v>1316</v>
       </c>
-      <c r="E58" s="2">
+      <c r="F58" s="2">
         <v>3508</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>45</v>
       </c>
       <c r="B59" s="2">
         <v>23293</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F59" s="2">
+        <v>24304</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>46</v>
       </c>
       <c r="B60" s="2">
         <v>1337</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F60" s="2">
+        <v>3368</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>47</v>
       </c>
       <c r="B61" s="2">
         <v>214608</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F61" s="2">
+        <v>222816</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H61" s="3">
+        <v>228109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -1656,7 +1777,7 @@
         <v>65678</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
running instances with new config
</commit_message>
<xml_diff>
--- a/hw1/Instances/Results.xlsx
+++ b/hw1/Instances/Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2855B43-35C1-42D4-BE6B-D143B00997C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED83AC6-7EB5-4719-BACB-0DBFF17E1212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="2088" windowWidth="12312" windowHeight="9396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8760" yWindow="1812" windowWidth="12048" windowHeight="9396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="203">
   <si>
     <t>br17.1.sop</t>
   </si>
@@ -208,120 +208,15 @@
     <t>rbg358a.sop</t>
   </si>
   <si>
-    <t>43.0</t>
-  </si>
-  <si>
-    <t>62.2</t>
-  </si>
-  <si>
-    <t>61.1</t>
-  </si>
-  <si>
-    <t>18561.0</t>
-  </si>
-  <si>
     <t>2125.0</t>
   </si>
   <si>
-    <t>10368.6</t>
-  </si>
-  <si>
-    <t>10344.8</t>
-  </si>
-  <si>
-    <t>best_log</t>
-  </si>
-  <si>
-    <t>avg_log</t>
-  </si>
-  <si>
     <t>best_exp</t>
   </si>
   <si>
     <t>avg_exp</t>
   </si>
   <si>
-    <t>45629.8</t>
-  </si>
-  <si>
-    <t>45869.9</t>
-  </si>
-  <si>
-    <t>48308.2</t>
-  </si>
-  <si>
-    <t>47997.6</t>
-  </si>
-  <si>
-    <t>62747.2</t>
-  </si>
-  <si>
-    <t>64289.1</t>
-  </si>
-  <si>
-    <t>28443.0</t>
-  </si>
-  <si>
-    <t>28551.0</t>
-  </si>
-  <si>
-    <t>83295.5</t>
-  </si>
-  <si>
-    <t>83310.0</t>
-  </si>
-  <si>
-    <t>2643.1</t>
-  </si>
-  <si>
-    <t>2619.2</t>
-  </si>
-  <si>
-    <t>394.5</t>
-  </si>
-  <si>
-    <t>387.0</t>
-  </si>
-  <si>
-    <t>2048.4</t>
-  </si>
-  <si>
-    <t>2140.4</t>
-  </si>
-  <si>
-    <t>1765.7</t>
-  </si>
-  <si>
-    <t>1761.8</t>
-  </si>
-  <si>
-    <t>435.7</t>
-  </si>
-  <si>
-    <t>411.0</t>
-  </si>
-  <si>
-    <t>481.3</t>
-  </si>
-  <si>
-    <t>1085.1</t>
-  </si>
-  <si>
-    <t>1468.1</t>
-  </si>
-  <si>
-    <t>1407.0</t>
-  </si>
-  <si>
-    <t>1427.5</t>
-  </si>
-  <si>
-    <t>2631.9</t>
-  </si>
-  <si>
-    <t>3155.7</t>
-  </si>
-  <si>
     <t>3163.4</t>
   </si>
   <si>
@@ -415,21 +310,9 @@
     <t>max_exp</t>
   </si>
   <si>
-    <t>59.4</t>
-  </si>
-  <si>
     <t>59.2</t>
   </si>
   <si>
-    <t>18558.0</t>
-  </si>
-  <si>
-    <t>max_log</t>
-  </si>
-  <si>
-    <t>2002.8</t>
-  </si>
-  <si>
     <t>73565.4</t>
   </si>
   <si>
@@ -437,6 +320,315 @@
   </si>
   <si>
     <t>121699.8</t>
+  </si>
+  <si>
+    <t>0.1416</t>
+  </si>
+  <si>
+    <t>0.1446</t>
+  </si>
+  <si>
+    <t>0.1496</t>
+  </si>
+  <si>
+    <t>min_time</t>
+  </si>
+  <si>
+    <t>avg_time</t>
+  </si>
+  <si>
+    <t>max_time</t>
+  </si>
+  <si>
+    <t>0.1107</t>
+  </si>
+  <si>
+    <t>0.11877</t>
+  </si>
+  <si>
+    <t>57.8</t>
+  </si>
+  <si>
+    <t>0.1077</t>
+  </si>
+  <si>
+    <t>0.116270</t>
+  </si>
+  <si>
+    <t>0.1625</t>
+  </si>
+  <si>
+    <t>18400.5</t>
+  </si>
+  <si>
+    <t>1.7354</t>
+  </si>
+  <si>
+    <t>1.7924</t>
+  </si>
+  <si>
+    <t>1.9119</t>
+  </si>
+  <si>
+    <t>4.1928</t>
+  </si>
+  <si>
+    <t>4.4230</t>
+  </si>
+  <si>
+    <t>4.6745</t>
+  </si>
+  <si>
+    <t>10312.8</t>
+  </si>
+  <si>
+    <t>1.1050</t>
+  </si>
+  <si>
+    <t>1.2013</t>
+  </si>
+  <si>
+    <t>1.3194</t>
+  </si>
+  <si>
+    <t>45597.4</t>
+  </si>
+  <si>
+    <t>2.0604</t>
+  </si>
+  <si>
+    <t>2.3552</t>
+  </si>
+  <si>
+    <t>2.7556</t>
+  </si>
+  <si>
+    <t>58427.8</t>
+  </si>
+  <si>
+    <t>4.9487</t>
+  </si>
+  <si>
+    <t>5.2376</t>
+  </si>
+  <si>
+    <t>5.4843</t>
+  </si>
+  <si>
+    <t>66684.35</t>
+  </si>
+  <si>
+    <t>2.9372</t>
+  </si>
+  <si>
+    <t>3.2266</t>
+  </si>
+  <si>
+    <t>3.4667</t>
+  </si>
+  <si>
+    <t>28598.75</t>
+  </si>
+  <si>
+    <t>0.8178</t>
+  </si>
+  <si>
+    <t>0.9116</t>
+  </si>
+  <si>
+    <t>1.0894</t>
+  </si>
+  <si>
+    <t>83270.5</t>
+  </si>
+  <si>
+    <t>0.3390</t>
+  </si>
+  <si>
+    <t>0.3805</t>
+  </si>
+  <si>
+    <t>0.4697</t>
+  </si>
+  <si>
+    <t>3870.05</t>
+  </si>
+  <si>
+    <t>4.0428</t>
+  </si>
+  <si>
+    <t>4.2812</t>
+  </si>
+  <si>
+    <t>4.5359</t>
+  </si>
+  <si>
+    <t>548.15</t>
+  </si>
+  <si>
+    <t>0.7549</t>
+  </si>
+  <si>
+    <t>0.8216</t>
+  </si>
+  <si>
+    <t>0.9136</t>
+  </si>
+  <si>
+    <t>2301.3</t>
+  </si>
+  <si>
+    <t>0.6532</t>
+  </si>
+  <si>
+    <t>0.7296</t>
+  </si>
+  <si>
+    <t>0.8986</t>
+  </si>
+  <si>
+    <t>2545.5</t>
+  </si>
+  <si>
+    <t>1.4327</t>
+  </si>
+  <si>
+    <t>1.5482</t>
+  </si>
+  <si>
+    <t>1.6655</t>
+  </si>
+  <si>
+    <t>2881.25</t>
+  </si>
+  <si>
+    <t>1.9058</t>
+  </si>
+  <si>
+    <t>2.1013</t>
+  </si>
+  <si>
+    <t>2.2778</t>
+  </si>
+  <si>
+    <t>439.4</t>
+  </si>
+  <si>
+    <t>0.8008</t>
+  </si>
+  <si>
+    <t>0.9093</t>
+  </si>
+  <si>
+    <t>1.0082</t>
+  </si>
+  <si>
+    <t>432.75</t>
+  </si>
+  <si>
+    <t>0.8028</t>
+  </si>
+  <si>
+    <t>0.9041</t>
+  </si>
+  <si>
+    <t>1.1270</t>
+  </si>
+  <si>
+    <t>480.9</t>
+  </si>
+  <si>
+    <t>0.7749</t>
+  </si>
+  <si>
+    <t>0.8580</t>
+  </si>
+  <si>
+    <t>0.9614</t>
+  </si>
+  <si>
+    <t>1104.55</t>
+  </si>
+  <si>
+    <t>1.9378</t>
+  </si>
+  <si>
+    <t>2.1143</t>
+  </si>
+  <si>
+    <t>2.4140</t>
+  </si>
+  <si>
+    <t>1450.35</t>
+  </si>
+  <si>
+    <t>1.8151</t>
+  </si>
+  <si>
+    <t>1.9227</t>
+  </si>
+  <si>
+    <t>2.1562</t>
+  </si>
+  <si>
+    <t>1397.25</t>
+  </si>
+  <si>
+    <t>1.8051</t>
+  </si>
+  <si>
+    <t>1.9065</t>
+  </si>
+  <si>
+    <t>2.0226</t>
+  </si>
+  <si>
+    <t>1421.6</t>
+  </si>
+  <si>
+    <t>1.9942</t>
+  </si>
+  <si>
+    <t>2.2430</t>
+  </si>
+  <si>
+    <t>2.6624</t>
+  </si>
+  <si>
+    <t>1801.35</t>
+  </si>
+  <si>
+    <t>2.1233</t>
+  </si>
+  <si>
+    <t>2.2379</t>
+  </si>
+  <si>
+    <t>2.4345</t>
+  </si>
+  <si>
+    <t>2605.35</t>
+  </si>
+  <si>
+    <t>6.6901</t>
+  </si>
+  <si>
+    <t>7.2614</t>
+  </si>
+  <si>
+    <t>7.8829</t>
+  </si>
+  <si>
+    <t>3140.35</t>
+  </si>
+  <si>
+    <t>8.1642</t>
+  </si>
+  <si>
+    <t>8.7001</t>
+  </si>
+  <si>
+    <t>9.8681</t>
   </si>
 </sst>
 </file>
@@ -446,7 +638,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-3000401]#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,13 +657,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B0F0"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -504,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -515,16 +700,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -811,985 +990,1192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.09765625" style="2"/>
-    <col min="3" max="3" width="8.796875" style="3"/>
-    <col min="4" max="7" width="8.796875" style="2"/>
-    <col min="8" max="8" width="8.796875" style="3"/>
+    <col min="3" max="5" width="8.796875" style="2"/>
+    <col min="6" max="9" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="1"/>
+      <c r="D1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>41</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="2">
         <v>41</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="2">
-        <v>41</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="E2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="3">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>55</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="2">
         <v>55</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="2">
-        <v>55</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H3" s="3">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="3">
+        <v>65</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>55</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="2">
         <v>55</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="2">
-        <v>55</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="E4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="3">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>18230</v>
       </c>
-      <c r="C5" s="3">
-        <v>18325</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="2">
-        <v>18325</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="3">
-        <v>18750</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>18250</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="3">
+        <v>18535</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>2125</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="2">
         <v>2125</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="3">
         <v>2125</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="3">
-        <v>2125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>8026</v>
       </c>
-      <c r="C7" s="3">
-        <v>9900</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="2">
-        <v>9581</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>9473</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="3">
+        <v>11041</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>40419</v>
       </c>
-      <c r="C8" s="3">
-        <v>44247</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="2">
-        <v>44128</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="D8" s="2">
+        <v>44076</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="3">
+        <v>46640</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>39420</v>
       </c>
-      <c r="C9" s="3">
-        <v>46722</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="2">
-        <v>46859</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="D9" s="2">
+        <v>53465</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="3">
+        <v>61435</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>49499</v>
       </c>
-      <c r="C10" s="3">
-        <v>58827</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="2">
-        <v>58699</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <v>62252</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="3">
+        <v>71833</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>28140</v>
       </c>
-      <c r="C11" s="3">
-        <v>28320</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="2">
-        <v>28305</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>28290</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="3">
+        <v>28810</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>83005</v>
       </c>
-      <c r="C12" s="3">
-        <v>83170</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="2">
-        <v>83170</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="D12" s="2">
+        <v>83140</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="3">
+        <v>83445</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>1123</v>
       </c>
-      <c r="C13" s="3">
-        <v>2372</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2201</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <v>3158</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4849</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>243</v>
       </c>
-      <c r="C14" s="3">
-        <v>346</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="2">
-        <v>353</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="D14" s="2">
+        <v>421</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="3">
+        <v>682</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>1071</v>
       </c>
-      <c r="C15" s="3">
-        <v>1699</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1714</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="D15" s="2">
+        <v>1788</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2981</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>912</v>
       </c>
-      <c r="C16" s="3">
-        <v>1625</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1610</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16" s="2">
+        <v>1952</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2968</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>879</v>
       </c>
-      <c r="F17" s="2">
-        <v>1757</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H17" s="3">
-        <v>2235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <v>2310</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3525</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>400</v>
       </c>
-      <c r="F18" s="2">
-        <v>411</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <v>407</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" s="3">
+        <v>478</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>397</v>
       </c>
-      <c r="F19" s="2">
-        <v>404</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <v>403</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F19" s="3">
+        <v>463</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>467</v>
       </c>
-      <c r="F20" s="2">
-        <v>469</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <v>468</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F20" s="3">
+        <v>494</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>1023</v>
       </c>
-      <c r="F21" s="2">
-        <v>1047</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <v>1064</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1143</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2">
         <v>1423</v>
       </c>
-      <c r="F22" s="2">
-        <v>1437</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <v>1424</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1507</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>1361</v>
       </c>
-      <c r="F23" s="2">
-        <v>1369</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <v>1366</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1436</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>1381</v>
       </c>
-      <c r="F24" s="2">
-        <v>1390</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="2">
+        <v>1398</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1481</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="2">
         <v>1765</v>
       </c>
-      <c r="F25" s="2">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="2">
+        <v>1774</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1832</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>2544</v>
       </c>
-      <c r="F26" s="2">
-        <v>2581</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <v>2578</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F26" s="3">
+        <v>2632</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="2">
         <v>3062</v>
       </c>
-      <c r="F27" s="2">
-        <v>3138</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <v>3101</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F27" s="3">
+        <v>3187</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="2">
         <v>2568</v>
       </c>
-      <c r="F28" s="2">
+      <c r="D28" s="2">
         <v>3125</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="2">
         <v>16666</v>
       </c>
-      <c r="F29" s="2">
+      <c r="D29" s="2">
         <v>18247</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>19894</v>
       </c>
-      <c r="F30" s="2">
+      <c r="D30" s="2">
         <v>21773</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="E30" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="2">
         <v>915</v>
       </c>
-      <c r="F31" s="2">
+      <c r="D31" s="2">
         <v>1598</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="E31" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="2">
         <v>198</v>
       </c>
-      <c r="F32" s="2">
+      <c r="D32" s="2">
         <v>1050</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>56</v>
       </c>
       <c r="B33" s="2">
         <v>1494</v>
       </c>
-      <c r="F33" s="2">
+      <c r="D33" s="2">
         <v>1497</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="2">
         <v>1750</v>
       </c>
-      <c r="F34" s="2">
+      <c r="D34" s="2">
         <v>1782</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="2">
         <v>2033</v>
       </c>
-      <c r="F35" s="2">
+      <c r="D35" s="2">
         <v>2062</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="2">
         <v>2241</v>
       </c>
-      <c r="F36" s="2">
+      <c r="D36" s="2">
         <v>2283</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
       <c r="B37" s="2">
         <v>3482</v>
       </c>
-      <c r="F37" s="2">
+      <c r="D37" s="2">
         <v>3561</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>61</v>
       </c>
       <c r="B38" s="2">
         <v>2545</v>
       </c>
-      <c r="F38" s="2">
+      <c r="D38" s="2">
         <v>2922</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E38" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>29</v>
       </c>
       <c r="B40" s="2">
         <v>1109</v>
       </c>
-      <c r="F40" s="2">
+      <c r="D40" s="2">
         <v>1111</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="2">
         <v>577</v>
       </c>
-      <c r="F41" s="2">
+      <c r="D41" s="2">
         <v>580</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
       <c r="B42" s="2">
         <v>791</v>
       </c>
-      <c r="F42" s="2">
+      <c r="D42" s="2">
         <v>797</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="2">
         <v>245</v>
       </c>
-      <c r="F43" s="2">
+      <c r="D43" s="2">
         <v>247</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
       <c r="B44" s="2">
         <v>1016</v>
       </c>
-      <c r="F44" s="2">
+      <c r="D44" s="2">
         <v>1022</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E44" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
       <c r="B45" s="2">
         <v>155</v>
       </c>
-      <c r="F45" s="2">
+      <c r="D45" s="2">
         <v>155</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E45" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
       <c r="B46" s="2">
         <v>64</v>
       </c>
-      <c r="F46" s="2">
+      <c r="D46" s="2">
         <v>65</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E46" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
       <c r="B47" s="2">
         <v>2018</v>
       </c>
-      <c r="F47" s="2">
+      <c r="D47" s="2">
         <v>2018</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E47" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
       <c r="B48" s="2">
         <v>3466</v>
       </c>
-      <c r="F48" s="2">
+      <c r="D48" s="2">
         <v>3466</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E48" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
       <c r="B49" s="2">
         <v>84</v>
       </c>
-      <c r="F49" s="2">
+      <c r="D49" s="2">
         <v>84</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E49" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
       <c r="B50" s="2">
         <v>127</v>
       </c>
-      <c r="F50" s="2">
+      <c r="D50" s="2">
         <v>127</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E50" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>38</v>
       </c>
       <c r="B52" s="2">
         <v>61</v>
       </c>
-      <c r="F52" s="2">
+      <c r="D52" s="2">
         <v>154</v>
       </c>
-      <c r="G52" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E52" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
       <c r="B53" s="2">
         <v>71749</v>
       </c>
-      <c r="F53" s="2">
+      <c r="D53" s="2">
         <v>73090</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H53" s="3">
+      <c r="E53" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F53" s="3">
         <v>74322</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>40</v>
       </c>
       <c r="B54" s="2">
         <v>41196</v>
       </c>
-      <c r="F54" s="2">
+      <c r="D54" s="2">
         <v>45481</v>
       </c>
-      <c r="G54" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E54" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="2">
         <v>71556</v>
       </c>
-      <c r="F55" s="2">
+      <c r="D55" s="2">
         <v>72943</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E55" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="2">
         <v>109471</v>
       </c>
-      <c r="F56" s="2">
+      <c r="D56" s="2">
         <v>112435</v>
       </c>
-      <c r="G56" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="E56" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B57" s="2">
         <v>38963</v>
       </c>
-      <c r="F57" s="2">
+      <c r="D57" s="2">
         <v>63323</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E57" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>44</v>
       </c>
       <c r="B58" s="2">
         <v>1316</v>
       </c>
-      <c r="F58" s="2">
+      <c r="D58" s="2">
         <v>3508</v>
       </c>
-      <c r="G58" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E58" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>45</v>
       </c>
       <c r="B59" s="2">
         <v>23293</v>
       </c>
-      <c r="F59" s="2">
+      <c r="D59" s="2">
         <v>24304</v>
       </c>
-      <c r="G59" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E59" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>46</v>
       </c>
       <c r="B60" s="2">
         <v>1337</v>
       </c>
-      <c r="F60" s="2">
+      <c r="D60" s="2">
         <v>3368</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>47</v>
       </c>
       <c r="B61" s="2">
         <v>214608</v>
       </c>
-      <c r="F61" s="2">
+      <c r="D61" s="2">
         <v>222816</v>
       </c>
-      <c r="G61" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H61" s="3">
+      <c r="E61" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F61" s="3">
         <v>228109</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
       <c r="B62" s="2">
         <v>65678</v>
       </c>
-      <c r="F62" s="2">
+      <c r="D62" s="2">
         <v>119694</v>
       </c>
-      <c r="G62" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H62" s="3">
+      <c r="E62" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F62" s="3">
         <v>123546</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>49</v>
       </c>

</xml_diff>